<commit_message>
appendix and readme updates
</commit_message>
<xml_diff>
--- a/supplemental_docs/spotify_vs_librosa_metrics.xlsx
+++ b/supplemental_docs/spotify_vs_librosa_metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Documents/GA-DSI/capstone/supplemental_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C41FA83-3477-834C-9E54-E7F519B7D769}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6521CA7D-2712-4C4B-B3B0-BF78E5412861}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2200" yWindow="-22920" windowWidth="33340" windowHeight="20880" xr2:uid="{DEA02990-78CA-374A-A733-D67231CB97DE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33340" windowHeight="20500" xr2:uid="{DEA02990-78CA-374A-A733-D67231CB97DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Spotify Metrics of Interest</t>
   </si>
@@ -61,12 +61,6 @@
   </si>
   <si>
     <t>librosa_score_t5</t>
-  </si>
-  <si>
-    <t>Independent Spotify MOI</t>
-  </si>
-  <si>
-    <t>Librosa Independent MOI</t>
   </si>
 </sst>
 </file>
@@ -429,8 +423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395E663A-2C0C-8B4E-A569-FD84A34E04BB}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -487,12 +481,8 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>